<commit_message>
'Avg_NI_loose', 'Sigma_NI_loose', 'Avg_Num_loose', 'Sigma_Num_loose'
'Avg_NI_loose', 'Sigma_NI_loose', 'Avg_Num_loose', 'Sigma_Num_loose'
</commit_message>
<xml_diff>
--- a/out_test/tables/aggregated_30.xlsx
+++ b/out_test/tables/aggregated_30.xlsx
@@ -777,76 +777,76 @@
         <v>10</v>
       </c>
       <c r="F2">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H2">
-        <v>47.3</v>
+        <v>48.1</v>
       </c>
       <c r="I2">
-        <v>17.84404662625605</v>
+        <v>22.3268896176785</v>
       </c>
       <c r="J2">
-        <v>0.4333333333333333</v>
+        <v>0.5</v>
       </c>
       <c r="K2">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="L2">
         <v>0.8</v>
       </c>
       <c r="M2">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="N2">
-        <v>0.4933333333333333</v>
+        <v>0.5166666666666666</v>
       </c>
       <c r="O2">
-        <v>0.7633333333333334</v>
+        <v>0.7533333333333333</v>
       </c>
       <c r="P2">
-        <v>0.640581346149906</v>
+        <v>0.6383947427798635</v>
       </c>
       <c r="Q2">
-        <v>0.02494438257849294</v>
+        <v>0.01666666666666666</v>
       </c>
       <c r="R2">
-        <v>0.02333333333333337</v>
+        <v>0.02666666666666671</v>
       </c>
       <c r="S2">
-        <v>0.004944310511912471</v>
+        <v>0.008744066132873943</v>
       </c>
       <c r="T2">
         <v>0.2</v>
       </c>
       <c r="U2">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="V2">
-        <v>0.5666666666666667</v>
+        <v>0.5</v>
       </c>
       <c r="W2">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="X2">
-        <v>0.2366666666666667</v>
+        <v>0.2466666666666667</v>
       </c>
       <c r="Y2">
-        <v>0.5066666666666666</v>
+        <v>0.4833333333333333</v>
       </c>
       <c r="Z2">
-        <v>0.3594186538500941</v>
+        <v>0.3616052572201364</v>
       </c>
       <c r="AA2">
-        <v>0.02333333333333333</v>
+        <v>0.02666666666666666</v>
       </c>
       <c r="AB2">
-        <v>0.02494438257849294</v>
+        <v>0.01666666666666666</v>
       </c>
       <c r="AC2">
-        <v>0.004944310511912416</v>
+        <v>0.008744066132873905</v>
       </c>
     </row>
     <row r="3" spans="1:62">
@@ -860,181 +860,181 @@
         <v>5</v>
       </c>
       <c r="D3">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="E3">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F3">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="G3">
-        <v>101</v>
+        <v>39</v>
       </c>
       <c r="H3">
-        <v>34.375</v>
+        <v>24.75</v>
       </c>
       <c r="I3">
-        <v>29.6687440752048</v>
+        <v>8.613216588476108</v>
       </c>
       <c r="J3">
-        <v>0.3333333333333333</v>
+        <v>0.4333333333333333</v>
       </c>
       <c r="K3">
         <v>0</v>
       </c>
       <c r="L3">
-        <v>0.8</v>
+        <v>0.7666666666666667</v>
       </c>
       <c r="M3">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="N3">
-        <v>0.475</v>
+        <v>0.4833333333333333</v>
       </c>
       <c r="O3">
-        <v>0.7375</v>
+        <v>0.75</v>
       </c>
       <c r="P3">
-        <v>0.6247947181993263</v>
+        <v>0.6325671185539604</v>
       </c>
       <c r="Q3">
-        <v>0.06180165405913052</v>
+        <v>0.03726779962499649</v>
       </c>
       <c r="R3">
-        <v>0.03510895738823486</v>
+        <v>0.01666666666666672</v>
       </c>
       <c r="S3">
-        <v>0.01154702497281603</v>
+        <v>0.01487283663062444</v>
       </c>
       <c r="T3">
-        <v>0.2</v>
+        <v>0.2333333333333333</v>
       </c>
       <c r="U3">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="V3">
-        <v>0.6666666666666666</v>
+        <v>0.5666666666666667</v>
       </c>
       <c r="W3">
         <v>0</v>
       </c>
       <c r="X3">
-        <v>0.2625</v>
+        <v>0.25</v>
       </c>
       <c r="Y3">
-        <v>0.525</v>
+        <v>0.5166666666666666</v>
       </c>
       <c r="Z3">
-        <v>0.3752052818006736</v>
+        <v>0.3674328814460394</v>
       </c>
       <c r="AA3">
-        <v>0.03510895738823482</v>
+        <v>0.01666666666666666</v>
       </c>
       <c r="AB3">
-        <v>0.06180165405913051</v>
+        <v>0.03726779962499649</v>
       </c>
       <c r="AC3">
-        <v>0.01154702497281599</v>
+        <v>0.01487283663062436</v>
       </c>
       <c r="AD3">
-        <v>-0.4242640687119285</v>
+        <v>-0.3713906763541082</v>
       </c>
       <c r="AE3">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="AF3">
-        <v>1.260656560172406</v>
+        <v>1.092252505352855</v>
       </c>
       <c r="AG3">
         <v>0</v>
       </c>
       <c r="AH3">
-        <v>-0.2350260367470899</v>
+        <v>-0.3185081647987705</v>
       </c>
       <c r="AI3">
-        <v>0.9200929122757008</v>
+        <v>0.8424401481062922</v>
       </c>
       <c r="AJ3">
-        <v>0.1465175320937149</v>
+        <v>0.1462867770181568</v>
       </c>
       <c r="AK3">
-        <v>0.1880907729945215</v>
+        <v>0.05388500430424849</v>
       </c>
       <c r="AL3">
-        <v>0.2167481180179686</v>
+        <v>0.1908172457089166</v>
       </c>
       <c r="AM3">
-        <v>0.09014496927549201</v>
+        <v>0.05013341473119987</v>
       </c>
       <c r="AN3">
-        <v>-2.385873333333322</v>
+        <v>-6.2084233333333</v>
       </c>
       <c r="AO3">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="AP3">
-        <v>44.49349333333333</v>
+        <v>31.90051666666668</v>
       </c>
       <c r="AQ3">
         <v>0</v>
       </c>
       <c r="AR3">
-        <v>-1.354672499999998</v>
+        <v>-3.244539999999994</v>
       </c>
       <c r="AS3">
-        <v>28.83540958333334</v>
+        <v>26.34928583333333</v>
       </c>
       <c r="AT3">
-        <v>2.423831992827272</v>
+        <v>2.075130786948432</v>
       </c>
       <c r="AU3">
+        <v>0.5</v>
+      </c>
+      <c r="AV3">
         <v>2</v>
       </c>
-      <c r="AV3">
-        <v>4</v>
-      </c>
       <c r="AW3">
-        <v>2.456547619047619</v>
+        <v>1.041666666666667</v>
       </c>
       <c r="AX3">
-        <v>1.25</v>
+        <v>1.071428571428571</v>
       </c>
       <c r="AY3">
-        <v>2.285714285714286</v>
+        <v>1.727272727272727</v>
       </c>
       <c r="AZ3">
-        <v>1.566464785214785</v>
+        <v>1.394751082251082</v>
       </c>
       <c r="BA3">
-        <v>1.061797949279874</v>
+        <v>1.167643096050927</v>
       </c>
       <c r="BB3">
-        <v>1.793068050937266</v>
+        <v>1.395156829017423</v>
       </c>
       <c r="BC3">
-        <v>1.323213740102504</v>
+        <v>1.261222096154614</v>
       </c>
       <c r="BD3">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="BE3">
-        <v>44</v>
+        <v>75</v>
       </c>
       <c r="BF3">
-        <v>33.5</v>
+        <v>37.5</v>
       </c>
       <c r="BG3">
-        <v>10.5</v>
+        <v>19.49145111751987</v>
       </c>
       <c r="BH3">
-        <v>101.8106</v>
+        <v>96.98199999999999</v>
       </c>
       <c r="BI3">
-        <v>1.009000000000015</v>
+        <v>5.90874027691182</v>
       </c>
       <c r="BJ3">
-        <v>102.8196</v>
+        <v>103.8361</v>
       </c>
     </row>
     <row r="4" spans="1:62">
@@ -1048,181 +1048,181 @@
         <v>5</v>
       </c>
       <c r="D4">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="E4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F4">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="G4">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="H4">
-        <v>40</v>
+        <v>43.83333333333334</v>
       </c>
       <c r="I4">
-        <v>34.57166469813104</v>
+        <v>35.22506998652459</v>
       </c>
       <c r="J4">
-        <v>0.4666666666666667</v>
+        <v>0.4</v>
       </c>
       <c r="K4">
         <v>0</v>
       </c>
       <c r="L4">
-        <v>0.8333333333333334</v>
+        <v>0.7666666666666667</v>
       </c>
       <c r="M4">
-        <v>97</v>
+        <v>19</v>
       </c>
       <c r="N4">
-        <v>0.48</v>
+        <v>0.4722222222222223</v>
       </c>
       <c r="O4">
-        <v>0.7533333333333333</v>
+        <v>0.7611111111111111</v>
       </c>
       <c r="P4">
-        <v>0.6341858387799564</v>
+        <v>0.6374740804183195</v>
       </c>
       <c r="Q4">
-        <v>0.01632993161855452</v>
+        <v>0.04044505494044732</v>
       </c>
       <c r="R4">
-        <v>0.04521553322083516</v>
+        <v>0.01242259987499887</v>
       </c>
       <c r="S4">
-        <v>0.01116127612780876</v>
+        <v>0.007378962604085104</v>
       </c>
       <c r="T4">
-        <v>0.1666666666666667</v>
+        <v>0.2333333333333333</v>
       </c>
       <c r="U4">
-        <v>97</v>
+        <v>19</v>
       </c>
       <c r="V4">
-        <v>0.5333333333333333</v>
+        <v>0.6</v>
       </c>
       <c r="W4">
         <v>0</v>
       </c>
       <c r="X4">
-        <v>0.2466666666666667</v>
+        <v>0.2388888888888889</v>
       </c>
       <c r="Y4">
-        <v>0.52</v>
+        <v>0.5277777777777778</v>
       </c>
       <c r="Z4">
-        <v>0.3658141612200435</v>
+        <v>0.3625259195816805</v>
       </c>
       <c r="AA4">
-        <v>0.04521553322083512</v>
+        <v>0.01242259987499883</v>
       </c>
       <c r="AB4">
-        <v>0.01632993161855452</v>
+        <v>0.04044505494044731</v>
       </c>
       <c r="AC4">
-        <v>0.01116127612780876</v>
+        <v>0.007378962604085149</v>
       </c>
       <c r="AD4">
-        <v>-0.4522670168666447</v>
+        <v>-0.5345224838248431</v>
       </c>
       <c r="AE4">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="AF4">
-        <v>1.040820074429404</v>
+        <v>1.185239731832779</v>
       </c>
       <c r="AG4">
         <v>0</v>
       </c>
       <c r="AH4">
-        <v>-0.2444712029823259</v>
+        <v>-0.3123860300252375</v>
       </c>
       <c r="AI4">
-        <v>0.9853479778818203</v>
+        <v>0.9004036577351888</v>
       </c>
       <c r="AJ4">
-        <v>0.1173078722756749</v>
+        <v>0.09318061711599511</v>
       </c>
       <c r="AK4">
-        <v>0.1818297166024355</v>
+        <v>0.1580683724567594</v>
       </c>
       <c r="AL4">
-        <v>0.04698270541690446</v>
+        <v>0.2056869798554296</v>
       </c>
       <c r="AM4">
-        <v>0.06742130205511511</v>
+        <v>0.05513687789923368</v>
       </c>
       <c r="AN4">
-        <v>-2.366943333333325</v>
+        <v>-4.383626666666672</v>
       </c>
       <c r="AO4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AP4">
-        <v>37.27512333333335</v>
+        <v>42.19244999999999</v>
       </c>
       <c r="AQ4">
         <v>0</v>
       </c>
       <c r="AR4">
-        <v>-1.072843333333336</v>
+        <v>-2.133382777777781</v>
       </c>
       <c r="AS4">
-        <v>34.03993266666667</v>
+        <v>30.15259166666667</v>
       </c>
       <c r="AT4">
-        <v>1.937864483071896</v>
+        <v>1.391999370091558</v>
       </c>
       <c r="AU4">
-        <v>1.5</v>
+        <v>0.875</v>
       </c>
       <c r="AV4">
-        <v>2</v>
+        <v>2.333333333333333</v>
       </c>
       <c r="AW4">
-        <v>1.783333333333334</v>
+        <v>1.548611111111111</v>
       </c>
       <c r="AX4">
-        <v>1.071428571428571</v>
+        <v>1.230769230769231</v>
       </c>
       <c r="AY4">
         <v>2</v>
       </c>
       <c r="AZ4">
-        <v>1.473260073260073</v>
+        <v>1.492826617826618</v>
       </c>
       <c r="BA4">
-        <v>1.069361063179038</v>
+        <v>1.064762139431568</v>
       </c>
       <c r="BB4">
-        <v>1.393103889650616</v>
+        <v>1.38629966509762</v>
       </c>
       <c r="BC4">
-        <v>1.229125974336219</v>
+        <v>1.172321505803338</v>
       </c>
       <c r="BD4">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="BE4">
-        <v>36</v>
+        <v>92</v>
       </c>
       <c r="BF4">
-        <v>29</v>
+        <v>55.5</v>
       </c>
       <c r="BG4">
-        <v>6.870225614927067</v>
+        <v>21.5</v>
       </c>
       <c r="BH4">
-        <v>96.99477999999999</v>
+        <v>100.7383</v>
       </c>
       <c r="BI4">
-        <v>7.057594923314883</v>
+        <v>3.839457477300663</v>
       </c>
       <c r="BJ4">
-        <v>104.4484</v>
+        <v>104.2441</v>
       </c>
     </row>
     <row r="5" spans="1:62">
@@ -1236,181 +1236,181 @@
         <v>5</v>
       </c>
       <c r="D5">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="E5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F5">
-        <v>70</v>
+        <v>25</v>
       </c>
       <c r="G5">
-        <v>74</v>
+        <v>92</v>
       </c>
       <c r="H5">
-        <v>72</v>
+        <v>47</v>
       </c>
       <c r="I5">
-        <v>2</v>
+        <v>23.68966019173766</v>
       </c>
       <c r="J5">
         <v>0.5</v>
       </c>
       <c r="K5">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="L5">
-        <v>0.8</v>
+        <v>0.7666666666666667</v>
       </c>
       <c r="M5">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="N5">
-        <v>0.5</v>
+        <v>0.5266666666666666</v>
       </c>
       <c r="O5">
-        <v>0.7666666666666666</v>
+        <v>0.74</v>
       </c>
       <c r="P5">
-        <v>0.6386638872344652</v>
+        <v>0.6372090434191499</v>
       </c>
       <c r="Q5">
-        <v>0</v>
+        <v>0.02494438257849294</v>
       </c>
       <c r="R5">
-        <v>0.03333333333333338</v>
+        <v>0.02494438257849298</v>
       </c>
       <c r="S5">
-        <v>0.002432003176493891</v>
+        <v>0.01199015347339989</v>
       </c>
       <c r="T5">
-        <v>0.2</v>
+        <v>0.2333333333333333</v>
       </c>
       <c r="U5">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="V5">
         <v>0.5</v>
       </c>
       <c r="W5">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="X5">
-        <v>0.2333333333333333</v>
+        <v>0.26</v>
       </c>
       <c r="Y5">
-        <v>0.5</v>
+        <v>0.4733333333333333</v>
       </c>
       <c r="Z5">
-        <v>0.361336112765535</v>
+        <v>0.3627909565808503</v>
       </c>
       <c r="AA5">
-        <v>0.03333333333333333</v>
+        <v>0.02494438257849294</v>
       </c>
       <c r="AB5">
-        <v>0</v>
+        <v>0.02494438257849294</v>
       </c>
       <c r="AC5">
-        <v>0.002432003176493919</v>
+        <v>0.01199015347339987</v>
       </c>
       <c r="AD5">
-        <v>-0.5883484054145462</v>
+        <v>-0.5380077714285122</v>
       </c>
       <c r="AE5">
-        <v>47</v>
+        <v>8</v>
       </c>
       <c r="AF5">
-        <v>0.5664327763538516</v>
+        <v>0.5294521438194486</v>
       </c>
       <c r="AG5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH5">
-        <v>-0.4912018042679816</v>
+        <v>-0.4044676856946253</v>
       </c>
       <c r="AI5">
-        <v>0.5599957744419215</v>
+        <v>0.4656792343549968</v>
       </c>
       <c r="AJ5">
-        <v>0.03856323406764888</v>
+        <v>0.06248502010570839</v>
       </c>
       <c r="AK5">
-        <v>0.09714660114656465</v>
+        <v>0.07120002421052611</v>
       </c>
       <c r="AL5">
-        <v>0.006437001911930029</v>
+        <v>0.0494898477811711</v>
       </c>
       <c r="AM5">
-        <v>0.0009117082010921679</v>
+        <v>0.02298281822734283</v>
       </c>
       <c r="AN5">
-        <v>-0.3490000000000002</v>
+        <v>-0.7042133333333389</v>
       </c>
       <c r="AO5">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AP5">
-        <v>4.610493333333331</v>
+        <v>4.44253333333333</v>
       </c>
       <c r="AQ5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR5">
-        <v>-0.2231749999999977</v>
+        <v>-0.3725226666666678</v>
       </c>
       <c r="AS5">
-        <v>3.745143333333331</v>
+        <v>3.601620666666664</v>
       </c>
       <c r="AT5">
-        <v>0.1010165432466414</v>
+        <v>0.150396703344872</v>
       </c>
       <c r="AU5">
+        <v>0</v>
+      </c>
+      <c r="AV5">
         <v>1.333333333333333</v>
       </c>
-      <c r="AV5">
-        <v>2</v>
-      </c>
       <c r="AW5">
-        <v>1.666666666666667</v>
+        <v>0.7666666666666666</v>
       </c>
       <c r="AX5">
         <v>1.071428571428571</v>
       </c>
       <c r="AY5">
-        <v>1.25</v>
+        <v>1.777777777777778</v>
       </c>
       <c r="AZ5">
-        <v>1.160714285714286</v>
+        <v>1.360750360750361</v>
       </c>
       <c r="BA5">
-        <v>1.04065027143127</v>
+        <v>1.03760678066032</v>
       </c>
       <c r="BB5">
-        <v>1.050189804481089</v>
+        <v>1.151143810076616</v>
       </c>
       <c r="BC5">
-        <v>1.04542003795618</v>
+        <v>1.096336852483821</v>
       </c>
       <c r="BD5">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="BE5">
-        <v>94</v>
+        <v>70</v>
       </c>
       <c r="BF5">
-        <v>40.125</v>
+        <v>51.8</v>
       </c>
       <c r="BG5">
-        <v>26.36966770742476</v>
+        <v>16.9162643630324</v>
       </c>
       <c r="BH5">
-        <v>25.7919375</v>
+        <v>25.88602</v>
       </c>
       <c r="BI5">
-        <v>0.5439301998820714</v>
+        <v>0.20659972313631</v>
       </c>
       <c r="BJ5">
-        <v>26.2128</v>
+        <v>26.1303</v>
       </c>
     </row>
     <row r="6" spans="1:62">
@@ -1424,181 +1424,181 @@
         <v>5</v>
       </c>
       <c r="D6">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="G6">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="H6">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="I6">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="J6">
-        <v>0.5</v>
+        <v>0.5333333333333333</v>
       </c>
       <c r="K6">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="L6">
-        <v>0.8</v>
+        <v>0.7333333333333333</v>
       </c>
       <c r="M6">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="N6">
-        <v>0.5166666666666666</v>
+        <v>0.5333333333333333</v>
       </c>
       <c r="O6">
-        <v>0.7666666666666666</v>
+        <v>0.7333333333333333</v>
       </c>
       <c r="P6">
-        <v>0.6445019553715206</v>
+        <v>0.6448979591836739</v>
       </c>
       <c r="Q6">
-        <v>0.01666666666666666</v>
+        <v>0</v>
       </c>
       <c r="R6">
-        <v>0.03333333333333338</v>
+        <v>0</v>
       </c>
       <c r="S6">
-        <v>0.006820795951230918</v>
+        <v>0</v>
       </c>
       <c r="T6">
-        <v>0.2</v>
+        <v>0.2666666666666667</v>
       </c>
       <c r="U6">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="V6">
-        <v>0.5</v>
+        <v>0.4666666666666667</v>
       </c>
       <c r="W6">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="X6">
-        <v>0.2333333333333333</v>
+        <v>0.2666666666666667</v>
       </c>
       <c r="Y6">
-        <v>0.4833333333333333</v>
+        <v>0.4666666666666667</v>
       </c>
       <c r="Z6">
-        <v>0.3554980446284794</v>
+        <v>0.3551020408163267</v>
       </c>
       <c r="AA6">
-        <v>0.03333333333333333</v>
+        <v>0</v>
       </c>
       <c r="AB6">
-        <v>0.01666666666666666</v>
+        <v>0</v>
       </c>
       <c r="AC6">
-        <v>0.006820795951230668</v>
+        <v>0</v>
       </c>
       <c r="AD6">
-        <v>-0.3527641774466536</v>
+        <v>-0.3333333333333272</v>
       </c>
       <c r="AE6">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="AF6">
-        <v>0.4711412405896289</v>
+        <v>0.4704462138528056</v>
       </c>
       <c r="AG6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH6">
-        <v>-0.2736605533420143</v>
+        <v>-0.3333333333333272</v>
       </c>
       <c r="AI6">
-        <v>0.4563939121954919</v>
+        <v>0.4704462138528056</v>
       </c>
       <c r="AJ6">
-        <v>0.08962252713485298</v>
+        <v>0.04177136173167684</v>
       </c>
       <c r="AK6">
-        <v>0.07910362410463929</v>
+        <v>0</v>
       </c>
       <c r="AL6">
-        <v>0.01474732839413703</v>
+        <v>0</v>
       </c>
       <c r="AM6">
-        <v>0.04015220226840132</v>
+        <v>0</v>
       </c>
       <c r="AN6">
-        <v>-0.1579533333333245</v>
+        <v>-0.1779600000000059</v>
       </c>
       <c r="AO6">
         <v>6</v>
       </c>
       <c r="AP6">
-        <v>3.713370000000003</v>
+        <v>3.956106666666667</v>
       </c>
       <c r="AQ6">
         <v>0</v>
       </c>
       <c r="AR6">
-        <v>-0.1462849999999953</v>
+        <v>-0.1779600000000059</v>
       </c>
       <c r="AS6">
-        <v>3.152933333333334</v>
+        <v>3.956106666666667</v>
       </c>
       <c r="AT6">
-        <v>0.188831256038647</v>
+        <v>0.09801129251700663</v>
       </c>
       <c r="AU6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AV6">
-        <v>2.333333333333333</v>
+        <v>0.5</v>
       </c>
       <c r="AW6">
-        <v>1.666666666666667</v>
+        <v>0.5</v>
       </c>
       <c r="AX6">
-        <v>1.307692307692308</v>
+        <v>1.454545454545455</v>
       </c>
       <c r="AY6">
-        <v>1.363636363636364</v>
+        <v>1.454545454545455</v>
       </c>
       <c r="AZ6">
-        <v>1.335664335664336</v>
+        <v>1.454545454545455</v>
       </c>
       <c r="BA6">
-        <v>1.091098600164078</v>
+        <v>1.148567037471385</v>
       </c>
       <c r="BB6">
-        <v>1.22004191072339</v>
+        <v>1.148567037471385</v>
       </c>
       <c r="BC6">
-        <v>1.155570255443734</v>
+        <v>1.148567037471385</v>
       </c>
       <c r="BD6">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="BE6">
-        <v>100</v>
+        <v>72</v>
       </c>
       <c r="BF6">
-        <v>53.125</v>
+        <v>40</v>
       </c>
       <c r="BG6">
-        <v>21.76831125742188</v>
+        <v>15.20233900132184</v>
       </c>
       <c r="BH6">
-        <v>25.5279125</v>
+        <v>25.86423333333333</v>
       </c>
       <c r="BI6">
-        <v>0.3461912709670043</v>
+        <v>0.3147881227464314</v>
       </c>
       <c r="BJ6">
-        <v>26.0028</v>
+        <v>26.2063</v>
       </c>
     </row>
     <row r="7" spans="1:62">
@@ -1612,181 +1612,181 @@
         <v>5</v>
       </c>
       <c r="D7">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="E7">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F7">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="G7">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="H7">
-        <v>48.8</v>
+        <v>29.85714285714286</v>
       </c>
       <c r="I7">
-        <v>29.3148426569204</v>
+        <v>27.07887195070077</v>
       </c>
       <c r="J7">
-        <v>0.4666666666666667</v>
+        <v>0.4333333333333333</v>
       </c>
       <c r="K7">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="L7">
         <v>0.8</v>
       </c>
       <c r="M7">
-        <v>28</v>
+        <v>78</v>
       </c>
       <c r="N7">
-        <v>0.4933333333333333</v>
+        <v>0.5</v>
       </c>
       <c r="O7">
-        <v>0.74</v>
+        <v>0.7333333333333334</v>
       </c>
       <c r="P7">
-        <v>0.6322212047212048</v>
+        <v>0.6262645185986148</v>
       </c>
       <c r="Q7">
-        <v>0.02494438257849294</v>
+        <v>0.03984095364447978</v>
       </c>
       <c r="R7">
-        <v>0.03887301263230204</v>
+        <v>0.03984095364447982</v>
       </c>
       <c r="S7">
-        <v>0.009146022054143686</v>
+        <v>0.01818278468502089</v>
       </c>
       <c r="T7">
         <v>0.2</v>
       </c>
       <c r="U7">
-        <v>28</v>
+        <v>78</v>
       </c>
       <c r="V7">
-        <v>0.5333333333333333</v>
+        <v>0.5666666666666667</v>
       </c>
       <c r="W7">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="X7">
-        <v>0.26</v>
+        <v>0.2666666666666667</v>
       </c>
       <c r="Y7">
-        <v>0.5066666666666666</v>
+        <v>0.5</v>
       </c>
       <c r="Z7">
-        <v>0.3677787952787954</v>
+        <v>0.3737354814013853</v>
       </c>
       <c r="AA7">
-        <v>0.03887301263230199</v>
+        <v>0.03984095364447978</v>
       </c>
       <c r="AB7">
-        <v>0.02494438257849294</v>
+        <v>0.03984095364447978</v>
       </c>
       <c r="AC7">
-        <v>0.009146022054143525</v>
+        <v>0.01818278468502091</v>
       </c>
       <c r="AD7">
-        <v>-0.4082482904638582</v>
+        <v>-0.4472135954999571</v>
       </c>
       <c r="AE7">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="AF7">
-        <v>0.9589265404395483</v>
+        <v>1.008300211025157</v>
       </c>
       <c r="AG7">
         <v>0</v>
       </c>
       <c r="AH7">
-        <v>-0.2824402347540773</v>
+        <v>-0.2276380027586381</v>
       </c>
       <c r="AI7">
-        <v>0.7660015495096</v>
+        <v>0.8416926424509787</v>
       </c>
       <c r="AJ7">
-        <v>0.09782723933016038</v>
+        <v>0.1634464722407949</v>
       </c>
       <c r="AK7">
-        <v>0.09479179042251709</v>
+        <v>0.169542405714942</v>
       </c>
       <c r="AL7">
-        <v>0.146211826710528</v>
+        <v>0.121943485048657</v>
       </c>
       <c r="AM7">
-        <v>0.04698700387774774</v>
+        <v>0.1048503212332592</v>
       </c>
       <c r="AN7">
-        <v>-0.3854277850972601</v>
+        <v>-0.6274973281045035</v>
       </c>
       <c r="AO7">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="AP7">
-        <v>2.94208561552043</v>
+        <v>3.979515170783908</v>
       </c>
       <c r="AQ7">
         <v>0</v>
       </c>
       <c r="AR7">
-        <v>-0.2213647586824024</v>
+        <v>-0.211580486281038</v>
       </c>
       <c r="AS7">
-        <v>2.482827784826299</v>
+        <v>2.881399137649348</v>
       </c>
       <c r="AT7">
-        <v>0.1719228937373702</v>
+        <v>0.3802735077415532</v>
       </c>
       <c r="AU7">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AV7">
-        <v>1.666666666666667</v>
+        <v>2.5</v>
       </c>
       <c r="AW7">
-        <v>1.123333333333334</v>
+        <v>1.547619047619047</v>
       </c>
       <c r="AX7">
-        <v>1.214285714285714</v>
+        <v>1.285714285714286</v>
       </c>
       <c r="AY7">
-        <v>1.454545454545455</v>
+        <v>2</v>
       </c>
       <c r="AZ7">
-        <v>1.318031968031968</v>
+        <v>1.551530612244898</v>
       </c>
       <c r="BA7">
-        <v>1.072562482929696</v>
+        <v>1.066574036001902</v>
       </c>
       <c r="BB7">
-        <v>1.352182956224272</v>
+        <v>1.539823384363614</v>
       </c>
       <c r="BC7">
-        <v>1.176072805394655</v>
+        <v>1.296254851644574</v>
       </c>
       <c r="BD7">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="BE7">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="BF7">
-        <v>18.8</v>
+        <v>30.66666666666667</v>
       </c>
       <c r="BG7">
-        <v>7.054076835419359</v>
+        <v>17.46106780494506</v>
       </c>
       <c r="BH7">
-        <v>11.67223763655707</v>
+        <v>12.01606885157712</v>
       </c>
       <c r="BI7">
-        <v>0.932546832615349</v>
+        <v>0.593028620630157</v>
       </c>
       <c r="BJ7">
-        <v>12.7751260120747</v>
+        <v>12.55350613666823</v>
       </c>
     </row>
     <row r="8" spans="1:62">
@@ -1800,181 +1800,181 @@
         <v>5</v>
       </c>
       <c r="D8">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="E8">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F8">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G8">
-        <v>37</v>
+        <v>94</v>
       </c>
       <c r="H8">
-        <v>21.5</v>
+        <v>39.5</v>
       </c>
       <c r="I8">
-        <v>8.05708797684788</v>
+        <v>31.94135250736888</v>
       </c>
       <c r="J8">
         <v>0.4666666666666667</v>
       </c>
       <c r="K8">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="L8">
         <v>0.8</v>
       </c>
       <c r="M8">
-        <v>7</v>
+        <v>73</v>
       </c>
       <c r="N8">
-        <v>0.5055555555555555</v>
+        <v>0.5083333333333333</v>
       </c>
       <c r="O8">
-        <v>0.7666666666666666</v>
+        <v>0.75</v>
       </c>
       <c r="P8">
-        <v>0.6360904172669999</v>
+        <v>0.6247981296090306</v>
       </c>
       <c r="Q8">
-        <v>0.02290614236454255</v>
+        <v>0.02763853991962833</v>
       </c>
       <c r="R8">
-        <v>0.03849001794597509</v>
+        <v>0.03726779962499654</v>
       </c>
       <c r="S8">
-        <v>0.01516371636365017</v>
+        <v>0.012142116498713</v>
       </c>
       <c r="T8">
         <v>0.2</v>
       </c>
       <c r="U8">
-        <v>7</v>
+        <v>73</v>
       </c>
       <c r="V8">
         <v>0.5333333333333333</v>
       </c>
       <c r="W8">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="X8">
-        <v>0.2333333333333334</v>
+        <v>0.25</v>
       </c>
       <c r="Y8">
-        <v>0.4944444444444445</v>
+        <v>0.4916666666666667</v>
       </c>
       <c r="Z8">
-        <v>0.3639095827329999</v>
+        <v>0.3752018703909694</v>
       </c>
       <c r="AA8">
-        <v>0.03849001794597504</v>
+        <v>0.03726779962499649</v>
       </c>
       <c r="AB8">
-        <v>0.02290614236454255</v>
+        <v>0.02763853991962833</v>
       </c>
       <c r="AC8">
-        <v>0.01516371636365008</v>
+        <v>0.01214211649871295</v>
       </c>
       <c r="AD8">
-        <v>-0.2959941012741295</v>
+        <v>-0.4364357804719895</v>
       </c>
       <c r="AE8">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="AF8">
-        <v>0.9039642141703439</v>
+        <v>0.8475193177303518</v>
       </c>
       <c r="AG8">
         <v>0</v>
       </c>
       <c r="AH8">
-        <v>-0.203492322958049</v>
+        <v>-0.3855129132570119</v>
       </c>
       <c r="AI8">
-        <v>0.7184605149580229</v>
+        <v>0.689223000418848</v>
       </c>
       <c r="AJ8">
-        <v>0.1377044280225535</v>
+        <v>0.09952774953702093</v>
       </c>
       <c r="AK8">
-        <v>0.06795124480246263</v>
+        <v>0.03792030008025462</v>
       </c>
       <c r="AL8">
-        <v>0.114380326021273</v>
+        <v>0.12054784805238</v>
       </c>
       <c r="AM8">
-        <v>0.03846936701853907</v>
+        <v>0.04584659409327286</v>
       </c>
       <c r="AN8">
-        <v>-0.2734222027219833</v>
+        <v>-0.1962706352010866</v>
       </c>
       <c r="AO8">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="AP8">
-        <v>3.492114360999398</v>
+        <v>2.915173375998355</v>
       </c>
       <c r="AQ8">
         <v>0</v>
       </c>
       <c r="AR8">
-        <v>-0.1561825419084369</v>
+        <v>-0.1306840903735726</v>
       </c>
       <c r="AS8">
-        <v>2.511270487584182</v>
+        <v>2.534671073215327</v>
       </c>
       <c r="AT8">
-        <v>0.2874164283958834</v>
+        <v>0.2374007781987527</v>
       </c>
       <c r="AU8">
         <v>1</v>
       </c>
       <c r="AV8">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AW8">
-        <v>1.768783068783069</v>
+        <v>2.7</v>
       </c>
       <c r="AX8">
-        <v>1.071428571428571</v>
+        <v>1.153846153846154</v>
       </c>
       <c r="AY8">
-        <v>1.636363636363636</v>
+        <v>1.818181818181818</v>
       </c>
       <c r="AZ8">
-        <v>1.231518481518481</v>
+        <v>1.544594294594295</v>
       </c>
       <c r="BA8">
-        <v>1.189089000576639</v>
+        <v>1.058716664138587</v>
       </c>
       <c r="BB8">
-        <v>1.307299189558281</v>
+        <v>1.419083798710471</v>
       </c>
       <c r="BC8">
-        <v>1.236299433848991</v>
+        <v>1.213127288913058</v>
       </c>
       <c r="BD8">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="BE8">
-        <v>42</v>
+        <v>150</v>
       </c>
       <c r="BF8">
-        <v>25</v>
+        <v>59.16666666666666</v>
       </c>
       <c r="BG8">
-        <v>9.974968671630002</v>
+        <v>44.87915873642118</v>
       </c>
       <c r="BH8">
-        <v>12.61162071907376</v>
+        <v>11.66394742715304</v>
       </c>
       <c r="BI8">
-        <v>0.2776457928548832</v>
+        <v>1.166666006732365</v>
       </c>
       <c r="BJ8">
-        <v>12.87129965752215</v>
+        <v>12.8391615976917</v>
       </c>
     </row>
     <row r="9" spans="1:62">
@@ -1988,181 +1988,160 @@
         <v>5</v>
       </c>
       <c r="D9">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E9">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F9">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G9">
-        <v>56</v>
+        <v>83</v>
       </c>
       <c r="H9">
-        <v>17</v>
+        <v>23.1</v>
       </c>
       <c r="I9">
-        <v>15.36229149573722</v>
+        <v>22.51865892987413</v>
       </c>
       <c r="J9">
+        <v>0.1333333333333333</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0.8</v>
+      </c>
+      <c r="M9">
+        <v>67</v>
+      </c>
+      <c r="N9">
+        <v>0.2933333333333333</v>
+      </c>
+      <c r="O9">
+        <v>0.7266666666666668</v>
+      </c>
+      <c r="P9">
+        <v>0.6340074295822143</v>
+      </c>
+      <c r="Q9">
+        <v>0.09977753031397177</v>
+      </c>
+      <c r="R9">
+        <v>0.0466666666666667</v>
+      </c>
+      <c r="S9">
+        <v>0.02099332237622237</v>
+      </c>
+      <c r="T9">
         <v>0.2</v>
       </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9">
-        <v>0.7666666666666667</v>
-      </c>
-      <c r="M9">
-        <v>10</v>
-      </c>
-      <c r="N9">
-        <v>0.3037037037037036</v>
-      </c>
-      <c r="O9">
-        <v>0.7074074074074074</v>
-      </c>
-      <c r="P9">
-        <v>0.6185816275631092</v>
-      </c>
-      <c r="Q9">
-        <v>0.04829038818668627</v>
-      </c>
-      <c r="R9">
-        <v>0.0561694477337152</v>
-      </c>
-      <c r="S9">
-        <v>0.04993241303787523</v>
-      </c>
-      <c r="T9">
-        <v>0.2333333333333333</v>
-      </c>
       <c r="U9">
-        <v>10</v>
+        <v>67</v>
       </c>
       <c r="V9">
-        <v>0.8</v>
+        <v>0.8666666666666667</v>
       </c>
       <c r="W9">
         <v>0</v>
       </c>
       <c r="X9">
-        <v>0.2925925925925926</v>
+        <v>0.2733333333333333</v>
       </c>
       <c r="Y9">
-        <v>0.6962962962962963</v>
+        <v>0.7066666666666667</v>
       </c>
       <c r="Z9">
-        <v>0.381418372436891</v>
+        <v>0.3659925704177856</v>
       </c>
       <c r="AA9">
-        <v>0.05616944773371519</v>
+        <v>0.04666666666666665</v>
       </c>
       <c r="AB9">
-        <v>0.0482903881866863</v>
+        <v>0.0997775303139718</v>
       </c>
       <c r="AC9">
-        <v>0.04993241303787518</v>
+        <v>0.02099332237622237</v>
       </c>
       <c r="AD9">
-        <v>-0.3713906763540988</v>
+        <v>-0.472866243743454</v>
       </c>
       <c r="AE9">
         <v>43</v>
       </c>
       <c r="AF9">
-        <v>2.662354895480724</v>
+        <v>2.716758779522179</v>
       </c>
       <c r="AG9">
         <v>0</v>
       </c>
       <c r="AH9">
-        <v>-0.06271162428508124</v>
+        <v>-0.153566175884159</v>
       </c>
       <c r="AI9">
-        <v>1.973903288544146</v>
+        <v>2.037286093423872</v>
       </c>
       <c r="AJ9">
-        <v>0.219057555793534</v>
+        <v>0.1641044986403082</v>
       </c>
       <c r="AK9">
-        <v>0.1604487904191574</v>
+        <v>0.1868917772004891</v>
       </c>
       <c r="AL9">
-        <v>0.3861158525795783</v>
+        <v>0.4425137220010397</v>
       </c>
       <c r="AM9">
-        <v>0.137295557218328</v>
+        <v>0.09454452329209866</v>
       </c>
       <c r="AN9">
-        <v>-374.6969397095236</v>
+        <v>-1337.383279999503</v>
       </c>
       <c r="AO9">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AP9">
-        <v>16371.42950842719</v>
+        <v>18499.16262754863</v>
       </c>
       <c r="AQ9">
         <v>0</v>
       </c>
       <c r="AR9">
-        <v>9.824099281752247</v>
+        <v>-255.3722558707486</v>
       </c>
       <c r="AS9">
-        <v>13318.69828861031</v>
+        <v>14019.619345847</v>
       </c>
       <c r="AT9">
-        <v>1471.68592199253</v>
+        <v>1007.610991651432</v>
       </c>
       <c r="AU9">
-        <v>1.285714285714286</v>
+        <v>1</v>
       </c>
       <c r="AV9">
-        <v>2.8</v>
+        <v>2.2</v>
       </c>
       <c r="AW9">
-        <v>1.877818477818478</v>
+        <v>1.573015873015873</v>
       </c>
       <c r="AX9">
-        <v>1.153846153846154</v>
+        <v>1.071428571428571</v>
       </c>
       <c r="AY9">
-        <v>2</v>
+        <v>2.111111111111111</v>
       </c>
       <c r="AZ9">
-        <v>1.488859905526572</v>
+        <v>1.498824786324787</v>
       </c>
       <c r="BA9">
-        <v>1.142089141741638</v>
+        <v>1.072148970308405</v>
       </c>
       <c r="BB9">
-        <v>3.406746031746032</v>
+        <v>2.737819241513823</v>
       </c>
       <c r="BC9">
-        <v>1.977519981566866</v>
-      </c>
-      <c r="BD9">
-        <v>62</v>
-      </c>
-      <c r="BE9">
-        <v>62</v>
-      </c>
-      <c r="BF9">
-        <v>62</v>
-      </c>
-      <c r="BG9">
-        <v>0</v>
-      </c>
-      <c r="BH9">
-        <v>25336.46648519111</v>
-      </c>
-      <c r="BI9">
-        <v>0</v>
-      </c>
-      <c r="BJ9">
-        <v>25336.46648519111</v>
+        <v>1.769682038355162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
'I_start', 'GR_start', 'Pr_start', 'Pr_min', 'NI_Pr_min',     'Pr_max', 'NI_Pr_max', 'Pr_avg', 'NI_Pr_avg'
'I_start', 'GR_start', 'Pr_start', 'Pr_min', 'NI_Pr_min',
    'Pr_max', 'NI_Pr_max', 'Pr_avg', 'NI_Pr_avg'
</commit_message>
<xml_diff>
--- a/out_test/tables/aggregated_30.xlsx
+++ b/out_test/tables/aggregated_30.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="81">
   <si>
     <t>Fitness Function</t>
   </si>
@@ -209,6 +209,33 @@
   </si>
   <si>
     <t>nonMax_F_found</t>
+  </si>
+  <si>
+    <t>I_start</t>
+  </si>
+  <si>
+    <t>GR_start</t>
+  </si>
+  <si>
+    <t>Pr_start</t>
+  </si>
+  <si>
+    <t>Pr_min</t>
+  </si>
+  <si>
+    <t>NI_Pr_min</t>
+  </si>
+  <si>
+    <t>Pr_max</t>
+  </si>
+  <si>
+    <t>NI_Pr_max</t>
+  </si>
+  <si>
+    <t>Pr_avg</t>
+  </si>
+  <si>
+    <t>NI_Pr_avg</t>
   </si>
   <si>
     <t>Fx2</t>
@@ -561,7 +588,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BJ9"/>
+  <dimension ref="A1:BS9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
@@ -572,7 +599,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:62">
+    <row r="1" spans="1:71">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -759,8 +786,35 @@
       <c r="BJ1" t="s">
         <v>64</v>
       </c>
+      <c r="BK1" t="s">
+        <v>65</v>
+      </c>
+      <c r="BL1" t="s">
+        <v>66</v>
+      </c>
+      <c r="BM1" t="s">
+        <v>67</v>
+      </c>
+      <c r="BN1" t="s">
+        <v>68</v>
+      </c>
+      <c r="BO1" t="s">
+        <v>69</v>
+      </c>
+      <c r="BP1" t="s">
+        <v>70</v>
+      </c>
+      <c r="BQ1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BR1" t="s">
+        <v>72</v>
+      </c>
+      <c r="BS1" t="s">
+        <v>73</v>
+      </c>
     </row>
-    <row r="2" spans="1:62">
+    <row r="2" spans="1:71">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -777,81 +831,81 @@
         <v>10</v>
       </c>
       <c r="F2">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="G2">
-        <v>89</v>
+        <v>118</v>
       </c>
       <c r="H2">
-        <v>48.1</v>
+        <v>43.3</v>
       </c>
       <c r="I2">
-        <v>22.3268896176785</v>
+        <v>27.90716753810748</v>
       </c>
       <c r="J2">
-        <v>0.5</v>
+        <v>0.4666666666666667</v>
       </c>
       <c r="K2">
-        <v>81</v>
+        <v>32</v>
       </c>
       <c r="L2">
-        <v>0.8</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="M2">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="N2">
-        <v>0.5166666666666666</v>
+        <v>0.5133333333333333</v>
       </c>
       <c r="O2">
-        <v>0.7533333333333333</v>
+        <v>0.7833333333333334</v>
       </c>
       <c r="P2">
-        <v>0.6383947427798635</v>
+        <v>0.6407892587843292</v>
       </c>
       <c r="Q2">
-        <v>0.01666666666666666</v>
+        <v>0.03055050463303893</v>
       </c>
       <c r="R2">
-        <v>0.02666666666666671</v>
+        <v>0.03073181485764299</v>
       </c>
       <c r="S2">
-        <v>0.008744066132873943</v>
+        <v>0.009170048688648527</v>
       </c>
       <c r="T2">
-        <v>0.2</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="U2">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="V2">
-        <v>0.5</v>
+        <v>0.5333333333333333</v>
       </c>
       <c r="W2">
-        <v>81</v>
+        <v>32</v>
       </c>
       <c r="X2">
-        <v>0.2466666666666667</v>
+        <v>0.2166666666666666</v>
       </c>
       <c r="Y2">
-        <v>0.4833333333333333</v>
+        <v>0.4866666666666666</v>
       </c>
       <c r="Z2">
-        <v>0.3616052572201364</v>
+        <v>0.3592107412156708</v>
       </c>
       <c r="AA2">
-        <v>0.02666666666666666</v>
+        <v>0.03073181485764296</v>
       </c>
       <c r="AB2">
-        <v>0.01666666666666666</v>
+        <v>0.03055050463303893</v>
       </c>
       <c r="AC2">
-        <v>0.008744066132873905</v>
+        <v>0.009170048688648508</v>
       </c>
     </row>
-    <row r="3" spans="1:62">
+    <row r="3" spans="1:71">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -860,25 +914,25 @@
         <v>5</v>
       </c>
       <c r="D3">
-        <v>0.4</v>
+        <v>0.7</v>
       </c>
       <c r="E3">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F3">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="G3">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H3">
-        <v>24.75</v>
+        <v>19.28571428571428</v>
       </c>
       <c r="I3">
-        <v>8.613216588476108</v>
+        <v>9.23834069384271</v>
       </c>
       <c r="J3">
-        <v>0.4333333333333333</v>
+        <v>0.4666666666666667</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -887,159 +941,159 @@
         <v>0.7666666666666667</v>
       </c>
       <c r="M3">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="N3">
-        <v>0.4833333333333333</v>
+        <v>0.5142857142857142</v>
       </c>
       <c r="O3">
-        <v>0.75</v>
+        <v>0.7238095238095238</v>
       </c>
       <c r="P3">
-        <v>0.6325671185539604</v>
+        <v>0.629366986860721</v>
       </c>
       <c r="Q3">
-        <v>0.03726779962499649</v>
+        <v>0.0301169300968417</v>
       </c>
       <c r="R3">
-        <v>0.01666666666666672</v>
+        <v>0.02935435239509038</v>
       </c>
       <c r="S3">
-        <v>0.01487283663062444</v>
+        <v>0.01148104871427595</v>
       </c>
       <c r="T3">
         <v>0.2333333333333333</v>
       </c>
       <c r="U3">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="V3">
-        <v>0.5666666666666667</v>
+        <v>0.5333333333333333</v>
       </c>
       <c r="W3">
         <v>0</v>
       </c>
       <c r="X3">
-        <v>0.25</v>
+        <v>0.2761904761904762</v>
       </c>
       <c r="Y3">
-        <v>0.5166666666666666</v>
+        <v>0.4857142857142858</v>
       </c>
       <c r="Z3">
-        <v>0.3674328814460394</v>
+        <v>0.3706330131392788</v>
       </c>
       <c r="AA3">
-        <v>0.01666666666666666</v>
+        <v>0.02935435239509036</v>
       </c>
       <c r="AB3">
-        <v>0.03726779962499649</v>
+        <v>0.0301169300968417</v>
       </c>
       <c r="AC3">
-        <v>0.01487283663062436</v>
+        <v>0.01148104871427597</v>
       </c>
       <c r="AD3">
-        <v>-0.3713906763541082</v>
+        <v>-0.4472135954999549</v>
       </c>
       <c r="AE3">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="AF3">
-        <v>1.092252505352855</v>
+        <v>0.9335618574477024</v>
       </c>
       <c r="AG3">
         <v>0</v>
       </c>
       <c r="AH3">
-        <v>-0.3185081647987705</v>
+        <v>-0.1689587167937017</v>
       </c>
       <c r="AI3">
-        <v>0.8424401481062922</v>
+        <v>0.7944406880994093</v>
       </c>
       <c r="AJ3">
-        <v>0.1462867770181568</v>
+        <v>0.1847841114813459</v>
       </c>
       <c r="AK3">
-        <v>0.05388500430424849</v>
+        <v>0.1350220098866607</v>
       </c>
       <c r="AL3">
-        <v>0.1908172457089166</v>
+        <v>0.1010014856140396</v>
       </c>
       <c r="AM3">
-        <v>0.05013341473119987</v>
+        <v>0.08681632988353034</v>
       </c>
       <c r="AN3">
-        <v>-6.2084233333333</v>
+        <v>-1.755359999999982</v>
       </c>
       <c r="AO3">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="AP3">
-        <v>31.90051666666668</v>
+        <v>34.17817</v>
       </c>
       <c r="AQ3">
         <v>0</v>
       </c>
       <c r="AR3">
-        <v>-3.244539999999994</v>
+        <v>-0.808959047619049</v>
       </c>
       <c r="AS3">
-        <v>26.34928583333333</v>
+        <v>25.12057333333334</v>
       </c>
       <c r="AT3">
-        <v>2.075130786948432</v>
+        <v>3.348877446634495</v>
       </c>
       <c r="AU3">
-        <v>0.5</v>
+        <v>1.25</v>
       </c>
       <c r="AV3">
-        <v>2</v>
+        <v>3.5</v>
       </c>
       <c r="AW3">
-        <v>1.041666666666667</v>
+        <v>2.083333333333333</v>
       </c>
       <c r="AX3">
-        <v>1.071428571428571</v>
+        <v>1.142857142857143</v>
       </c>
       <c r="AY3">
-        <v>1.727272727272727</v>
+        <v>1.7</v>
       </c>
       <c r="AZ3">
-        <v>1.394751082251082</v>
+        <v>1.395145330859616</v>
       </c>
       <c r="BA3">
-        <v>1.167643096050927</v>
+        <v>1.14267114068985</v>
       </c>
       <c r="BB3">
-        <v>1.395156829017423</v>
+        <v>1.64924907910056</v>
       </c>
       <c r="BC3">
-        <v>1.261222096154614</v>
+        <v>1.349008544567483</v>
       </c>
       <c r="BD3">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="BE3">
+        <v>84</v>
+      </c>
+      <c r="BF3">
+        <v>46</v>
+      </c>
+      <c r="BG3">
+        <v>30.24345659257001</v>
+      </c>
+      <c r="BH3">
+        <v>98.28500000000001</v>
+      </c>
+      <c r="BI3">
+        <v>2.070008004815445</v>
+      </c>
+      <c r="BJ3">
+        <v>101.2036</v>
+      </c>
+    </row>
+    <row r="4" spans="1:71">
+      <c r="A4" t="s">
         <v>75</v>
-      </c>
-      <c r="BF3">
-        <v>37.5</v>
-      </c>
-      <c r="BG3">
-        <v>19.49145111751987</v>
-      </c>
-      <c r="BH3">
-        <v>96.98199999999999</v>
-      </c>
-      <c r="BI3">
-        <v>5.90874027691182</v>
-      </c>
-      <c r="BJ3">
-        <v>103.8361</v>
-      </c>
-    </row>
-    <row r="4" spans="1:62">
-      <c r="A4" t="s">
-        <v>66</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -1048,22 +1102,22 @@
         <v>5</v>
       </c>
       <c r="D4">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
         <v>6</v>
       </c>
-      <c r="F4">
-        <v>13</v>
-      </c>
       <c r="G4">
-        <v>119</v>
+        <v>19</v>
       </c>
       <c r="H4">
-        <v>43.83333333333334</v>
+        <v>13.75</v>
       </c>
       <c r="I4">
-        <v>35.22506998652459</v>
+        <v>4.968651728587948</v>
       </c>
       <c r="J4">
         <v>0.4</v>
@@ -1075,31 +1129,31 @@
         <v>0.7666666666666667</v>
       </c>
       <c r="M4">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="N4">
-        <v>0.4722222222222223</v>
+        <v>0.4666666666666667</v>
       </c>
       <c r="O4">
-        <v>0.7611111111111111</v>
+        <v>0.7083333333333334</v>
       </c>
       <c r="P4">
-        <v>0.6374740804183195</v>
+        <v>0.6273842592592591</v>
       </c>
       <c r="Q4">
-        <v>0.04044505494044732</v>
+        <v>0.06236095644623234</v>
       </c>
       <c r="R4">
-        <v>0.01242259987499887</v>
+        <v>0.04930066485916349</v>
       </c>
       <c r="S4">
-        <v>0.007378962604085104</v>
+        <v>0.02184462912255682</v>
       </c>
       <c r="T4">
         <v>0.2333333333333333</v>
       </c>
       <c r="U4">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="V4">
         <v>0.6</v>
@@ -1108,126 +1162,126 @@
         <v>0</v>
       </c>
       <c r="X4">
-        <v>0.2388888888888889</v>
+        <v>0.2916666666666667</v>
       </c>
       <c r="Y4">
-        <v>0.5277777777777778</v>
+        <v>0.5333333333333334</v>
       </c>
       <c r="Z4">
-        <v>0.3625259195816805</v>
+        <v>0.3726157407407407</v>
       </c>
       <c r="AA4">
-        <v>0.01242259987499883</v>
+        <v>0.04930066485916346</v>
       </c>
       <c r="AB4">
-        <v>0.04044505494044731</v>
+        <v>0.06236095644623234</v>
       </c>
       <c r="AC4">
-        <v>0.007378962604085149</v>
+        <v>0.02184462912255688</v>
       </c>
       <c r="AD4">
-        <v>-0.5345224838248431</v>
+        <v>-0.2672612419124286</v>
       </c>
       <c r="AE4">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="AF4">
-        <v>1.185239731832779</v>
+        <v>1.138311383561731</v>
       </c>
       <c r="AG4">
         <v>0</v>
       </c>
       <c r="AH4">
-        <v>-0.3123860300252375</v>
+        <v>-0.1158443442626539</v>
       </c>
       <c r="AI4">
-        <v>0.9004036577351888</v>
+        <v>0.870841071022863</v>
       </c>
       <c r="AJ4">
-        <v>0.09318061711599511</v>
+        <v>0.2115753070435697</v>
       </c>
       <c r="AK4">
-        <v>0.1580683724567594</v>
+        <v>0.2230849638347916</v>
       </c>
       <c r="AL4">
-        <v>0.2056869798554296</v>
+        <v>0.2036004814567418</v>
       </c>
       <c r="AM4">
-        <v>0.05513687789923368</v>
+        <v>0.1451383908754069</v>
       </c>
       <c r="AN4">
-        <v>-4.383626666666672</v>
+        <v>-1.444053333333343</v>
       </c>
       <c r="AO4">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="AP4">
-        <v>42.19244999999999</v>
+        <v>40.52188333333332</v>
       </c>
       <c r="AQ4">
         <v>0</v>
       </c>
       <c r="AR4">
-        <v>-2.133382777777781</v>
+        <v>-0.3075066666666721</v>
       </c>
       <c r="AS4">
-        <v>30.15259166666667</v>
+        <v>28.16479</v>
       </c>
       <c r="AT4">
-        <v>1.391999370091558</v>
+        <v>4.033278769675928</v>
       </c>
       <c r="AU4">
-        <v>0.875</v>
+        <v>1.5</v>
       </c>
       <c r="AV4">
         <v>2.333333333333333</v>
       </c>
       <c r="AW4">
-        <v>1.548611111111111</v>
+        <v>2</v>
       </c>
       <c r="AX4">
-        <v>1.230769230769231</v>
+        <v>1.25</v>
       </c>
       <c r="AY4">
-        <v>2</v>
+        <v>1.666666666666667</v>
       </c>
       <c r="AZ4">
-        <v>1.492826617826618</v>
+        <v>1.49702380952381</v>
       </c>
       <c r="BA4">
-        <v>1.064762139431568</v>
+        <v>1.265662717628662</v>
       </c>
       <c r="BB4">
-        <v>1.38629966509762</v>
+        <v>1.610930735930736</v>
       </c>
       <c r="BC4">
-        <v>1.172321505803338</v>
+        <v>1.395729457958314</v>
       </c>
       <c r="BD4">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="BE4">
-        <v>92</v>
+        <v>58</v>
       </c>
       <c r="BF4">
-        <v>55.5</v>
+        <v>32.83333333333334</v>
       </c>
       <c r="BG4">
-        <v>21.5</v>
+        <v>15.48565644574215</v>
       </c>
       <c r="BH4">
-        <v>100.7383</v>
+        <v>101.5038</v>
       </c>
       <c r="BI4">
-        <v>3.839457477300663</v>
+        <v>3.551982468988263</v>
       </c>
       <c r="BJ4">
-        <v>104.2441</v>
+        <v>104.4484</v>
       </c>
     </row>
-    <row r="5" spans="1:62">
+    <row r="5" spans="1:71">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
@@ -1236,186 +1290,186 @@
         <v>5</v>
       </c>
       <c r="D5">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="E5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F5">
         <v>25</v>
       </c>
       <c r="G5">
-        <v>92</v>
+        <v>25</v>
       </c>
       <c r="H5">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="I5">
-        <v>23.68966019173766</v>
+        <v>0</v>
       </c>
       <c r="J5">
         <v>0.5</v>
       </c>
       <c r="K5">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="L5">
         <v>0.7666666666666667</v>
       </c>
       <c r="M5">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="N5">
-        <v>0.5266666666666666</v>
+        <v>0.5</v>
       </c>
       <c r="O5">
-        <v>0.74</v>
+        <v>0.7666666666666667</v>
       </c>
       <c r="P5">
-        <v>0.6372090434191499</v>
+        <v>0.6402777777777773</v>
       </c>
       <c r="Q5">
-        <v>0.02494438257849294</v>
+        <v>0</v>
       </c>
       <c r="R5">
-        <v>0.02494438257849298</v>
+        <v>0</v>
       </c>
       <c r="S5">
-        <v>0.01199015347339989</v>
+        <v>0</v>
       </c>
       <c r="T5">
         <v>0.2333333333333333</v>
       </c>
       <c r="U5">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="V5">
         <v>0.5</v>
       </c>
       <c r="W5">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="X5">
-        <v>0.26</v>
+        <v>0.2333333333333333</v>
       </c>
       <c r="Y5">
-        <v>0.4733333333333333</v>
+        <v>0.5</v>
       </c>
       <c r="Z5">
-        <v>0.3627909565808503</v>
+        <v>0.3597222222222221</v>
       </c>
       <c r="AA5">
-        <v>0.02494438257849294</v>
+        <v>0</v>
       </c>
       <c r="AB5">
-        <v>0.02494438257849294</v>
+        <v>0</v>
       </c>
       <c r="AC5">
-        <v>0.01199015347339987</v>
+        <v>0</v>
       </c>
       <c r="AD5">
-        <v>-0.5380077714285122</v>
+        <v>-0.2716340464031189</v>
       </c>
       <c r="AE5">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="AF5">
-        <v>0.5294521438194486</v>
+        <v>0.3573404598775777</v>
       </c>
       <c r="AG5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AH5">
-        <v>-0.4044676856946253</v>
+        <v>-0.2716340464031189</v>
       </c>
       <c r="AI5">
-        <v>0.4656792343549968</v>
+        <v>0.3573404598775777</v>
       </c>
       <c r="AJ5">
-        <v>0.06248502010570839</v>
+        <v>0.091630711971551</v>
       </c>
       <c r="AK5">
-        <v>0.07120002421052611</v>
+        <v>0</v>
       </c>
       <c r="AL5">
-        <v>0.0494898477811711</v>
+        <v>0</v>
       </c>
       <c r="AM5">
-        <v>0.02298281822734283</v>
+        <v>0</v>
       </c>
       <c r="AN5">
-        <v>-0.7042133333333389</v>
+        <v>-0.4107666666666603</v>
       </c>
       <c r="AO5">
         <v>8</v>
       </c>
       <c r="AP5">
-        <v>4.44253333333333</v>
+        <v>2.194673333333323</v>
       </c>
       <c r="AQ5">
         <v>0</v>
       </c>
       <c r="AR5">
-        <v>-0.3725226666666678</v>
+        <v>-0.4107666666666603</v>
       </c>
       <c r="AS5">
-        <v>3.601620666666664</v>
+        <v>2.194673333333323</v>
       </c>
       <c r="AT5">
-        <v>0.150396703344872</v>
+        <v>0.2258518055555555</v>
       </c>
       <c r="AU5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AV5">
-        <v>1.333333333333333</v>
+        <v>4</v>
       </c>
       <c r="AW5">
-        <v>0.7666666666666666</v>
+        <v>4</v>
       </c>
       <c r="AX5">
-        <v>1.071428571428571</v>
+        <v>1.142857142857143</v>
       </c>
       <c r="AY5">
-        <v>1.777777777777778</v>
+        <v>1.142857142857143</v>
       </c>
       <c r="AZ5">
-        <v>1.360750360750361</v>
+        <v>1.142857142857143</v>
       </c>
       <c r="BA5">
-        <v>1.03760678066032</v>
+        <v>1.221241720776046</v>
       </c>
       <c r="BB5">
-        <v>1.151143810076616</v>
+        <v>1.221241720776046</v>
       </c>
       <c r="BC5">
-        <v>1.096336852483821</v>
+        <v>1.221241720776046</v>
       </c>
       <c r="BD5">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="BE5">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="BF5">
-        <v>51.8</v>
+        <v>35.66666666666666</v>
       </c>
       <c r="BG5">
-        <v>16.9162643630324</v>
+        <v>7.195677714974301</v>
       </c>
       <c r="BH5">
-        <v>25.88602</v>
+        <v>25.76465555555556</v>
       </c>
       <c r="BI5">
-        <v>0.20659972313631</v>
+        <v>0.5321779174321958</v>
       </c>
       <c r="BJ5">
-        <v>26.1303</v>
+        <v>26.2095</v>
       </c>
     </row>
-    <row r="6" spans="1:62">
+    <row r="6" spans="1:71">
       <c r="A6" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
@@ -1430,13 +1484,13 @@
         <v>1</v>
       </c>
       <c r="F6">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="G6">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="H6">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -1445,13 +1499,13 @@
         <v>0.5333333333333333</v>
       </c>
       <c r="K6">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="L6">
         <v>0.7333333333333333</v>
       </c>
       <c r="M6">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="N6">
         <v>0.5333333333333333</v>
@@ -1460,7 +1514,7 @@
         <v>0.7333333333333333</v>
       </c>
       <c r="P6">
-        <v>0.6448979591836739</v>
+        <v>0.6285714285714286</v>
       </c>
       <c r="Q6">
         <v>0</v>
@@ -1475,13 +1529,13 @@
         <v>0.2666666666666667</v>
       </c>
       <c r="U6">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="V6">
         <v>0.4666666666666667</v>
       </c>
       <c r="W6">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="X6">
         <v>0.2666666666666667</v>
@@ -1490,7 +1544,7 @@
         <v>0.4666666666666667</v>
       </c>
       <c r="Z6">
-        <v>0.3551020408163267</v>
+        <v>0.3714285714285714</v>
       </c>
       <c r="AA6">
         <v>0</v>
@@ -1502,25 +1556,25 @@
         <v>0</v>
       </c>
       <c r="AD6">
-        <v>-0.3333333333333272</v>
+        <v>-0.2672612419124233</v>
       </c>
       <c r="AE6">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="AF6">
-        <v>0.4704462138528056</v>
+        <v>0.5394493729499837</v>
       </c>
       <c r="AG6">
         <v>0</v>
       </c>
       <c r="AH6">
-        <v>-0.3333333333333272</v>
+        <v>-0.2672612419124233</v>
       </c>
       <c r="AI6">
-        <v>0.4704462138528056</v>
+        <v>0.5394493729499837</v>
       </c>
       <c r="AJ6">
-        <v>0.04177136173167684</v>
+        <v>0.08661680856193768</v>
       </c>
       <c r="AK6">
         <v>0</v>
@@ -1532,78 +1586,78 @@
         <v>0</v>
       </c>
       <c r="AN6">
-        <v>-0.1779600000000059</v>
+        <v>-0.09739333333333278</v>
       </c>
       <c r="AO6">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AP6">
-        <v>3.956106666666667</v>
+        <v>4.014329999999998</v>
       </c>
       <c r="AQ6">
         <v>0</v>
       </c>
       <c r="AR6">
-        <v>-0.1779600000000059</v>
+        <v>-0.09739333333333278</v>
       </c>
       <c r="AS6">
-        <v>3.956106666666667</v>
+        <v>4.014329999999998</v>
       </c>
       <c r="AT6">
-        <v>0.09801129251700663</v>
+        <v>0.1995103174603172</v>
       </c>
       <c r="AU6">
-        <v>0.5</v>
+        <v>1.333333333333333</v>
       </c>
       <c r="AV6">
-        <v>0.5</v>
+        <v>1.333333333333333</v>
       </c>
       <c r="AW6">
-        <v>0.5</v>
+        <v>1.333333333333333</v>
       </c>
       <c r="AX6">
-        <v>1.454545454545455</v>
+        <v>1.666666666666667</v>
       </c>
       <c r="AY6">
-        <v>1.454545454545455</v>
+        <v>1.666666666666667</v>
       </c>
       <c r="AZ6">
-        <v>1.454545454545455</v>
+        <v>1.666666666666667</v>
       </c>
       <c r="BA6">
-        <v>1.148567037471385</v>
+        <v>1.219730212923289</v>
       </c>
       <c r="BB6">
-        <v>1.148567037471385</v>
+        <v>1.219730212923289</v>
       </c>
       <c r="BC6">
-        <v>1.148567037471385</v>
+        <v>1.219730212923289</v>
       </c>
       <c r="BD6">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="BE6">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="BF6">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="BG6">
-        <v>15.20233900132184</v>
+        <v>14.45298892578587</v>
       </c>
       <c r="BH6">
-        <v>25.86423333333333</v>
+        <v>26.04505555555556</v>
       </c>
       <c r="BI6">
-        <v>0.3147881227464314</v>
+        <v>0.2306164353356322</v>
       </c>
       <c r="BJ6">
-        <v>26.2063</v>
+        <v>26.214</v>
       </c>
     </row>
-    <row r="7" spans="1:62">
+    <row r="7" spans="1:71">
       <c r="A7" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
@@ -1618,16 +1672,16 @@
         <v>7</v>
       </c>
       <c r="F7">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="G7">
-        <v>92</v>
+        <v>51</v>
       </c>
       <c r="H7">
-        <v>29.85714285714286</v>
+        <v>26.14285714285714</v>
       </c>
       <c r="I7">
-        <v>27.07887195070077</v>
+        <v>11.48201788423435</v>
       </c>
       <c r="J7">
         <v>0.4333333333333333</v>
@@ -1636,34 +1690,34 @@
         <v>0</v>
       </c>
       <c r="L7">
-        <v>0.8</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="M7">
-        <v>78</v>
+        <v>18</v>
       </c>
       <c r="N7">
         <v>0.5</v>
       </c>
       <c r="O7">
-        <v>0.7333333333333334</v>
+        <v>0.7476190476190476</v>
       </c>
       <c r="P7">
-        <v>0.6262645185986148</v>
+        <v>0.6329663802042721</v>
       </c>
       <c r="Q7">
         <v>0.03984095364447978</v>
       </c>
       <c r="R7">
-        <v>0.03984095364447982</v>
+        <v>0.04312088161017821</v>
       </c>
       <c r="S7">
-        <v>0.01818278468502089</v>
+        <v>0.01883259148257703</v>
       </c>
       <c r="T7">
-        <v>0.2</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="U7">
-        <v>78</v>
+        <v>18</v>
       </c>
       <c r="V7">
         <v>0.5666666666666667</v>
@@ -1672,126 +1726,126 @@
         <v>0</v>
       </c>
       <c r="X7">
-        <v>0.2666666666666667</v>
+        <v>0.2523809523809524</v>
       </c>
       <c r="Y7">
         <v>0.5</v>
       </c>
       <c r="Z7">
-        <v>0.3737354814013853</v>
+        <v>0.3670336197957279</v>
       </c>
       <c r="AA7">
-        <v>0.03984095364447978</v>
+        <v>0.04312088161017817</v>
       </c>
       <c r="AB7">
         <v>0.03984095364447978</v>
       </c>
       <c r="AC7">
-        <v>0.01818278468502091</v>
+        <v>0.01883259148257703</v>
       </c>
       <c r="AD7">
-        <v>-0.4472135954999571</v>
+        <v>-0.6260990336999432</v>
       </c>
       <c r="AE7">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="AF7">
-        <v>1.008300211025157</v>
+        <v>1.044730758145375</v>
       </c>
       <c r="AG7">
         <v>0</v>
       </c>
       <c r="AH7">
-        <v>-0.2276380027586381</v>
+        <v>-0.3266510367701438</v>
       </c>
       <c r="AI7">
-        <v>0.8416926424509787</v>
+        <v>0.7608342700839471</v>
       </c>
       <c r="AJ7">
-        <v>0.1634464722407949</v>
+        <v>0.1294460671849579</v>
       </c>
       <c r="AK7">
-        <v>0.169542405714942</v>
+        <v>0.2111330763597631</v>
       </c>
       <c r="AL7">
-        <v>0.121943485048657</v>
+        <v>0.2218190598857689</v>
       </c>
       <c r="AM7">
-        <v>0.1048503212332592</v>
+        <v>0.06084630787185441</v>
       </c>
       <c r="AN7">
-        <v>-0.6274973281045035</v>
+        <v>-0.5827034033488996</v>
       </c>
       <c r="AO7">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="AP7">
-        <v>3.979515170783908</v>
+        <v>3.987087503295393</v>
       </c>
       <c r="AQ7">
         <v>0</v>
       </c>
       <c r="AR7">
-        <v>-0.211580486281038</v>
+        <v>-0.2662260940487088</v>
       </c>
       <c r="AS7">
-        <v>2.881399137649348</v>
+        <v>2.605776549483541</v>
       </c>
       <c r="AT7">
-        <v>0.3802735077415532</v>
+        <v>0.2617465281169628</v>
       </c>
       <c r="AU7">
         <v>1</v>
       </c>
       <c r="AV7">
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
       <c r="AW7">
-        <v>1.547619047619047</v>
+        <v>1.952380952380953</v>
       </c>
       <c r="AX7">
-        <v>1.285714285714286</v>
+        <v>1.071428571428571</v>
       </c>
       <c r="AY7">
-        <v>2</v>
+        <v>1.727272727272727</v>
       </c>
       <c r="AZ7">
-        <v>1.551530612244898</v>
+        <v>1.309761666904524</v>
       </c>
       <c r="BA7">
-        <v>1.066574036001902</v>
+        <v>1.122760574031826</v>
       </c>
       <c r="BB7">
-        <v>1.539823384363614</v>
+        <v>1.412061368583108</v>
       </c>
       <c r="BC7">
-        <v>1.296254851644574</v>
+        <v>1.245228450812102</v>
       </c>
       <c r="BD7">
         <v>12</v>
       </c>
       <c r="BE7">
-        <v>54</v>
+        <v>23</v>
       </c>
       <c r="BF7">
-        <v>30.66666666666667</v>
+        <v>18.33333333333333</v>
       </c>
       <c r="BG7">
-        <v>17.46106780494506</v>
+        <v>4.642796092394707</v>
       </c>
       <c r="BH7">
-        <v>12.01606885157712</v>
+        <v>12.56508030928504</v>
       </c>
       <c r="BI7">
-        <v>0.593028620630157</v>
+        <v>0.1669771511528002</v>
       </c>
       <c r="BJ7">
-        <v>12.55350613666823</v>
+        <v>12.7751260120747</v>
       </c>
     </row>
-    <row r="8" spans="1:62">
+    <row r="8" spans="1:71">
       <c r="A8" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
@@ -1800,186 +1854,186 @@
         <v>5</v>
       </c>
       <c r="D8">
-        <v>0.4</v>
+        <v>0.7</v>
       </c>
       <c r="E8">
+        <v>7</v>
+      </c>
+      <c r="F8">
+        <v>11</v>
+      </c>
+      <c r="G8">
+        <v>47</v>
+      </c>
+      <c r="H8">
+        <v>26.42857142857143</v>
+      </c>
+      <c r="I8">
+        <v>13.605221086639</v>
+      </c>
+      <c r="J8">
+        <v>0.3666666666666666</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0.7666666666666667</v>
+      </c>
+      <c r="M8">
+        <v>22</v>
+      </c>
+      <c r="N8">
+        <v>0.4619047619047619</v>
+      </c>
+      <c r="O8">
+        <v>0.7333333333333334</v>
+      </c>
+      <c r="P8">
+        <v>0.6317208912550527</v>
+      </c>
+      <c r="Q8">
+        <v>0.05172752614857246</v>
+      </c>
+      <c r="R8">
+        <v>0.02519763153394852</v>
+      </c>
+      <c r="S8">
+        <v>0.01384427692673933</v>
+      </c>
+      <c r="T8">
+        <v>0.2333333333333333</v>
+      </c>
+      <c r="U8">
+        <v>22</v>
+      </c>
+      <c r="V8">
+        <v>0.6333333333333333</v>
+      </c>
+      <c r="W8">
+        <v>0</v>
+      </c>
+      <c r="X8">
+        <v>0.2666666666666667</v>
+      </c>
+      <c r="Y8">
+        <v>0.5380952380952381</v>
+      </c>
+      <c r="Z8">
+        <v>0.3682791087449474</v>
+      </c>
+      <c r="AA8">
+        <v>0.02519763153394848</v>
+      </c>
+      <c r="AB8">
+        <v>0.05172752614857244</v>
+      </c>
+      <c r="AC8">
+        <v>0.01384427692673926</v>
+      </c>
+      <c r="AD8">
+        <v>-0.301511344577761</v>
+      </c>
+      <c r="AE8">
+        <v>18</v>
+      </c>
+      <c r="AF8">
+        <v>1.331112309523567</v>
+      </c>
+      <c r="AG8">
+        <v>0</v>
+      </c>
+      <c r="AH8">
+        <v>-0.1859865817609799</v>
+      </c>
+      <c r="AI8">
+        <v>0.8594240746038307</v>
+      </c>
+      <c r="AJ8">
+        <v>0.1440340745601538</v>
+      </c>
+      <c r="AK8">
+        <v>0.1205021261204545</v>
+      </c>
+      <c r="AL8">
+        <v>0.2771359123615238</v>
+      </c>
+      <c r="AM8">
+        <v>0.07967467399671466</v>
+      </c>
+      <c r="AN8">
+        <v>-0.3629278927530741</v>
+      </c>
+      <c r="AO8">
         <v>4</v>
       </c>
-      <c r="F8">
-        <v>15</v>
-      </c>
-      <c r="G8">
-        <v>94</v>
-      </c>
-      <c r="H8">
-        <v>39.5</v>
-      </c>
-      <c r="I8">
-        <v>31.94135250736888</v>
-      </c>
-      <c r="J8">
-        <v>0.4666666666666667</v>
-      </c>
-      <c r="K8">
-        <v>11</v>
-      </c>
-      <c r="L8">
-        <v>0.8</v>
-      </c>
-      <c r="M8">
-        <v>73</v>
-      </c>
-      <c r="N8">
-        <v>0.5083333333333333</v>
-      </c>
-      <c r="O8">
-        <v>0.75</v>
-      </c>
-      <c r="P8">
-        <v>0.6247981296090306</v>
-      </c>
-      <c r="Q8">
-        <v>0.02763853991962833</v>
-      </c>
-      <c r="R8">
-        <v>0.03726779962499654</v>
-      </c>
-      <c r="S8">
-        <v>0.012142116498713</v>
-      </c>
-      <c r="T8">
-        <v>0.2</v>
-      </c>
-      <c r="U8">
-        <v>73</v>
-      </c>
-      <c r="V8">
-        <v>0.5333333333333333</v>
-      </c>
-      <c r="W8">
-        <v>11</v>
-      </c>
-      <c r="X8">
-        <v>0.25</v>
-      </c>
-      <c r="Y8">
-        <v>0.4916666666666667</v>
-      </c>
-      <c r="Z8">
-        <v>0.3752018703909694</v>
-      </c>
-      <c r="AA8">
-        <v>0.03726779962499649</v>
-      </c>
-      <c r="AB8">
-        <v>0.02763853991962833</v>
-      </c>
-      <c r="AC8">
-        <v>0.01214211649871295</v>
-      </c>
-      <c r="AD8">
-        <v>-0.4364357804719895</v>
-      </c>
-      <c r="AE8">
-        <v>37</v>
-      </c>
-      <c r="AF8">
-        <v>0.8475193177303518</v>
-      </c>
-      <c r="AG8">
-        <v>0</v>
-      </c>
-      <c r="AH8">
-        <v>-0.3855129132570119</v>
-      </c>
-      <c r="AI8">
-        <v>0.689223000418848</v>
-      </c>
-      <c r="AJ8">
-        <v>0.09952774953702093</v>
-      </c>
-      <c r="AK8">
-        <v>0.03792030008025462</v>
-      </c>
-      <c r="AL8">
-        <v>0.12054784805238</v>
-      </c>
-      <c r="AM8">
-        <v>0.04584659409327286</v>
-      </c>
-      <c r="AN8">
-        <v>-0.1962706352010866</v>
-      </c>
-      <c r="AO8">
-        <v>10</v>
-      </c>
       <c r="AP8">
-        <v>2.915173375998355</v>
+        <v>5.142234990415643</v>
       </c>
       <c r="AQ8">
         <v>0</v>
       </c>
       <c r="AR8">
-        <v>-0.1306840903735726</v>
+        <v>-0.1505890620682873</v>
       </c>
       <c r="AS8">
-        <v>2.534671073215327</v>
+        <v>3.113724104230941</v>
       </c>
       <c r="AT8">
-        <v>0.2374007781987527</v>
+        <v>0.2592604396277233</v>
       </c>
       <c r="AU8">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="AV8">
-        <v>5</v>
+        <v>2.666666666666667</v>
       </c>
       <c r="AW8">
-        <v>2.7</v>
+        <v>1.521428571428571</v>
       </c>
       <c r="AX8">
-        <v>1.153846153846154</v>
+        <v>1.214285714285714</v>
       </c>
       <c r="AY8">
-        <v>1.818181818181818</v>
+        <v>2.142857142857143</v>
       </c>
       <c r="AZ8">
-        <v>1.544594294594295</v>
+        <v>1.581484388627246</v>
       </c>
       <c r="BA8">
-        <v>1.058716664138587</v>
+        <v>1.103802218131759</v>
       </c>
       <c r="BB8">
-        <v>1.419083798710471</v>
+        <v>1.416413807886822</v>
       </c>
       <c r="BC8">
-        <v>1.213127288913058</v>
+        <v>1.239574326910607</v>
       </c>
       <c r="BD8">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="BE8">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="BF8">
-        <v>59.16666666666666</v>
+        <v>66</v>
       </c>
       <c r="BG8">
-        <v>44.87915873642118</v>
+        <v>53.10994884827763</v>
       </c>
       <c r="BH8">
-        <v>11.66394742715304</v>
+        <v>12.79655125188746</v>
       </c>
       <c r="BI8">
-        <v>1.166666006732365</v>
+        <v>0.05443566557333544</v>
       </c>
       <c r="BJ8">
-        <v>12.8391615976917</v>
+        <v>12.87129965752215</v>
       </c>
     </row>
-    <row r="9" spans="1:62">
+    <row r="9" spans="1:71">
       <c r="A9" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="B9" t="s">
         <v>4</v>
@@ -1994,154 +2048,154 @@
         <v>10</v>
       </c>
       <c r="F9">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G9">
-        <v>83</v>
+        <v>26</v>
       </c>
       <c r="H9">
-        <v>23.1</v>
+        <v>13.4</v>
       </c>
       <c r="I9">
-        <v>22.51865892987413</v>
+        <v>6.62117814289874</v>
       </c>
       <c r="J9">
-        <v>0.1333333333333333</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="K9">
         <v>0</v>
       </c>
       <c r="L9">
-        <v>0.8</v>
+        <v>0.7666666666666667</v>
       </c>
       <c r="M9">
-        <v>67</v>
+        <v>17</v>
       </c>
       <c r="N9">
-        <v>0.2933333333333333</v>
+        <v>0.2733333333333333</v>
       </c>
       <c r="O9">
-        <v>0.7266666666666668</v>
+        <v>0.7100000000000001</v>
       </c>
       <c r="P9">
-        <v>0.6340074295822143</v>
+        <v>0.6187609161793372</v>
       </c>
       <c r="Q9">
-        <v>0.09977753031397177</v>
+        <v>0.08137703743822468</v>
       </c>
       <c r="R9">
-        <v>0.0466666666666667</v>
+        <v>0.05385164807134506</v>
       </c>
       <c r="S9">
-        <v>0.02099332237622237</v>
+        <v>0.03199143434196162</v>
       </c>
       <c r="T9">
-        <v>0.2</v>
+        <v>0.2333333333333333</v>
       </c>
       <c r="U9">
-        <v>67</v>
+        <v>17</v>
       </c>
       <c r="V9">
-        <v>0.8666666666666667</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="W9">
         <v>0</v>
       </c>
       <c r="X9">
-        <v>0.2733333333333333</v>
+        <v>0.29</v>
       </c>
       <c r="Y9">
-        <v>0.7066666666666667</v>
+        <v>0.7266666666666667</v>
       </c>
       <c r="Z9">
-        <v>0.3659925704177856</v>
+        <v>0.3812390838206627</v>
       </c>
       <c r="AA9">
-        <v>0.04666666666666665</v>
+        <v>0.05385164807134504</v>
       </c>
       <c r="AB9">
-        <v>0.0997775303139718</v>
+        <v>0.08137703743822471</v>
       </c>
       <c r="AC9">
-        <v>0.02099332237622237</v>
+        <v>0.03199143434196165</v>
       </c>
       <c r="AD9">
-        <v>-0.472866243743454</v>
+        <v>-0.5555555555555652</v>
       </c>
       <c r="AE9">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="AF9">
-        <v>2.716758779522179</v>
+        <v>2.803450351682867</v>
       </c>
       <c r="AG9">
         <v>0</v>
       </c>
       <c r="AH9">
-        <v>-0.153566175884159</v>
+        <v>-0.1015641634996209</v>
       </c>
       <c r="AI9">
-        <v>2.037286093423872</v>
+        <v>2.052914799399319</v>
       </c>
       <c r="AJ9">
-        <v>0.1641044986403082</v>
+        <v>0.2191458751788855</v>
       </c>
       <c r="AK9">
-        <v>0.1868917772004891</v>
+        <v>0.2437634036316809</v>
       </c>
       <c r="AL9">
-        <v>0.4425137220010397</v>
+        <v>0.44632251936433</v>
       </c>
       <c r="AM9">
-        <v>0.09454452329209866</v>
+        <v>0.1037733160951575</v>
       </c>
       <c r="AN9">
-        <v>-1337.383279999503</v>
+        <v>-1386.117119070754</v>
       </c>
       <c r="AO9">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AP9">
-        <v>18499.16262754863</v>
+        <v>16955.58364152483</v>
       </c>
       <c r="AQ9">
         <v>0</v>
       </c>
       <c r="AR9">
-        <v>-255.3722558707486</v>
+        <v>-124.8353237970266</v>
       </c>
       <c r="AS9">
-        <v>14019.619345847</v>
+        <v>14100.72419980129</v>
       </c>
       <c r="AT9">
-        <v>1007.610991651432</v>
+        <v>1232.478016019306</v>
       </c>
       <c r="AU9">
-        <v>1</v>
+        <v>0.7777777777777778</v>
       </c>
       <c r="AV9">
-        <v>2.2</v>
+        <v>2.4</v>
       </c>
       <c r="AW9">
-        <v>1.573015873015873</v>
+        <v>1.495854700854701</v>
       </c>
       <c r="AX9">
-        <v>1.071428571428571</v>
+        <v>1.214285714285714</v>
       </c>
       <c r="AY9">
-        <v>2.111111111111111</v>
+        <v>1.9</v>
       </c>
       <c r="AZ9">
-        <v>1.498824786324787</v>
+        <v>1.518479853479854</v>
       </c>
       <c r="BA9">
-        <v>1.072148970308405</v>
+        <v>1.243426787116279</v>
       </c>
       <c r="BB9">
-        <v>2.737819241513823</v>
+        <v>3.420952380952381</v>
       </c>
       <c r="BC9">
-        <v>1.769682038355162</v>
+        <v>1.976608515242893</v>
       </c>
     </row>
   </sheetData>

</xml_diff>